<commit_message>
file structure update hours update
</commit_message>
<xml_diff>
--- a/status reports/davy.xlsx
+++ b/status reports/davy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -227,6 +227,50 @@
   </si>
   <si>
     <t>Design and Decision Meeting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/14/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Encoder speed requirement calculation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/15/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ordered control system components</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Researched QNX installation methods and issues</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/14/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/13/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Researched sterilizable motor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/18/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Group Meeting on Skype</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gravity Compensation motor experiment</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -594,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1012,6 +1056,72 @@
       </c>
       <c r="C37" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38">
+        <v>1.5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>0.5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>0.5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update add receipts add motor rma
</commit_message>
<xml_diff>
--- a/status reports/davy.xlsx
+++ b/status reports/davy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -179,6 +179,10 @@
   </si>
   <si>
     <t>QNX - Interrupts</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RMA/ship motor/encoder</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -552,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1168,6 +1172,17 @@
       </c>
       <c r="C55" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="4">
+        <v>40245</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update add receipts
</commit_message>
<xml_diff>
--- a/status reports/davy.xlsx
+++ b/status reports/davy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -199,6 +199,14 @@
   </si>
   <si>
     <t>Group Meeting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OMAP UART documentation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>QNX 3D implementation design</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -572,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1265,6 +1273,28 @@
       </c>
       <c r="C62" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="4">
+        <v>40256</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="4">
+        <v>40259</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update finance update
</commit_message>
<xml_diff>
--- a/status reports/davy.xlsx
+++ b/status reports/davy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -235,6 +235,14 @@
   </si>
   <si>
     <t>AVR-CAN interface</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>beagleboard avr-can interface</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Group Meeting</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -608,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1444,6 +1452,50 @@
       </c>
       <c r="C75" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="4">
+        <v>40272</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="4">
+        <v>40273</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="4">
+        <v>40274</v>
+      </c>
+      <c r="B78">
+        <v>1.5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="4">
+        <v>40274</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update src update
</commit_message>
<xml_diff>
--- a/status reports/davy.xlsx
+++ b/status reports/davy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -243,6 +243,26 @@
   </si>
   <si>
     <t>Group Meeting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>buying parts for interface board</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>interface board soldering and assembly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>interface board debug</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pair programming with Erica</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>serial interface debug</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -616,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1496,6 +1516,72 @@
       </c>
       <c r="C79" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="4">
+        <v>40275</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="4">
+        <v>40277</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="4">
+        <v>40277</v>
+      </c>
+      <c r="B82">
+        <v>6.5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="4">
+        <v>40278</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="4">
+        <v>40279</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="4">
+        <v>40279</v>
+      </c>
+      <c r="B85">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>